<commit_message>
re-made migration (sqlite limitations) added user to booking model added booking view model added book controller moved populate to home added buttons to rooms
</commit_message>
<xml_diff>
--- a/Other/KazanHotels.xslx.xlsx
+++ b/Other/KazanHotels.xslx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\BookingSiteApp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C518F1-2D91-4B74-93CF-7EE255144020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B3F70C-BBBD-44A2-86E7-DE78B2B01C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F04B87FB-41DF-467C-A675-371A7F9933D6}"/>
   </bookViews>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E195DBA6-13D8-4B91-8657-53348AF91B79}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,8 +890,8 @@
         <v>49.1158</v>
       </c>
       <c r="M2" t="str">
-        <f>CONCATENATE("repository.Add&lt;HotelModel&gt;(new HotelModel { Name = """,A2,""", Address = """,G2,""", City = """,H2,""", Stars = ",B2," } );")</f>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Bulak", Address = "49 Pravo Bulachnaya", City = "Kazan Russia", Stars = 4 } );</v>
+        <f>CONCATENATE("repository.Add(new HotelModel { Name = """,A2,""", Address = """,G2,""", City = """,H2,""", Stars = ",B2," } );")</f>
+        <v>repository.Add(new HotelModel { Name = "Bulak", Address = "49 Pravo Bulachnaya", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -923,8 +923,8 @@
         <v>49.1937</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M53" si="0">CONCATENATE("repository.Add&lt;HotelModel&gt;(new HotelModel { Name = """,A3,""", Address = """,G3,""", City = """,H3,""", Stars = ",B3," } );")</f>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Tranzit", Address = "Highway Moscow ufa 812 km", City = "Kazan Russia", Stars = 3 } );</v>
+        <f t="shared" ref="M3:M53" si="0">CONCATENATE("repository.Add(new HotelModel { Name = """,A3,""", Address = """,G3,""", City = """,H3,""", Stars = ",B3," } );")</f>
+        <v>repository.Add(new HotelModel { Name = "Hotel Tranzit", Address = "Highway Moscow ufa 812 km", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Regina Hotel Kazan", Address = "11 50 Let Oktyabrya street", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Regina Hotel Kazan", Address = "11 50 Let Oktyabrya street", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Safyan", Address = "Ulitsa Safyan 6", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Safyan", Address = "Ulitsa Safyan 6", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Vostok Guest House", Address = "Ulitsa Novo-Davlikeevskaya 19", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Vostok Guest House", Address = "Ulitsa Novo-Davlikeevskaya 19", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Zebra Hostel", Address = "Fatykha Amirkhana Prospect 18A", City = "Kazan Russia", Stars = 1 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Zebra Hostel", Address = "Fatykha Amirkhana Prospect 18A", City = "Kazan Russia", Stars = 1 } );</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Luciano Spa Complex", Address = "Ostrovskogo Street 26", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Luciano Spa Complex", Address = "Ostrovskogo Street 26", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Mirage Hotel Kazan", Address = "Moskovskaya Street 1A", City = "Kazan Russia", Stars = 5 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Mirage Hotel Kazan", Address = "Moskovskaya Street 1A", City = "Kazan Russia", Stars = 5 } );</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Shalyapin Palace", Address = "University Street 7/80", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Shalyapin Palace", Address = "University Street 7/80", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hayall Hotel", Address = "Universitetskaya Street 16", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hayall Hotel", Address = "Universitetskaya Street 16", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Riviera Kazan", Address = "1A Fatkin Amirkhana Street", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel Riviera Kazan", Address = "1A Fatkin Amirkhana Street", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Art Hotel Kazan", Address = "Ostrowski Street 33", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Art Hotel Kazan", Address = "Ostrowski Street 33", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Korston Hotel &amp; Mall Kazan", Address = "North Ershova Street 1A", City = "Kazan Russia", Stars = 5 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Korston Hotel &amp; Mall Kazan", Address = "North Ershova Street 1A", City = "Kazan Russia", Stars = 5 } );</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Grand Hotel Kazan", Address = "Ulice Petersburg 1", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Grand Hotel Kazan", Address = "Ulice Petersburg 1", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Dunai Hotel", Address = "Bolotnikova Street 9", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Dunai Hotel", Address = "Bolotnikova Street 9", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Premium Hotel", Address = "Maksima Gorkogo Street 3", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Premium Hotel", Address = "Maksima Gorkogo Street 3", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Bon Ami", Address = "Ulice Ostrovsky House 31", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel Bon Ami", Address = "Ulice Ostrovsky House 31", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Osobnyak Na Teatralnoy", Address = "Teatralnaya Street 3", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Osobnyak Na Teatralnoy", Address = "Teatralnaya Street 3", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Gulf Stream Hotel", Address = "2nd Azinskaya Street 1G", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Gulf Stream Hotel", Address = "2nd Azinskaya Street 1G", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Best Eastern Novinka Hotel", Address = "Korolenko Street 30", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Best Eastern Novinka Hotel", Address = "Korolenko Street 30", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Ibis Kazan Centre", Address = "Pravo-Bulachnaya Street 43/1", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel Ibis Kazan Centre", Address = "Pravo-Bulachnaya Street 43/1", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Giuseppe", Address = "Kremlin 15/25", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel Giuseppe", Address = "Kremlin 15/25", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Park Inn Kazan", Address = "Ulitsa Lesgafta 9-11", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Park Inn Kazan", Address = "Ulitsa Lesgafta 9-11", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Suleiman Palace Hotel", Address = "Peterburgskaya Street 55", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Suleiman Palace Hotel", Address = "Peterburgskaya Street 55", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Ilmar City Hotel Kazan", Address = "Karbysheva Street 12A", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Ilmar City Hotel Kazan", Address = "Karbysheva Street 12A", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "IT-Park Hotel", Address = "Peterburgskaya Street 52", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "IT-Park Hotel", Address = "Peterburgskaya Street 52", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Milena Hotel Kazan", Address = "19 Tazi Gizatta Street", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Milena Hotel Kazan", Address = "19 Tazi Gizatta Street", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Regina na Peterburgskoy", Address = "Peterburgskaya Street 11", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Regina na Peterburgskoy", Address = "Peterburgskaya Street 11", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1932,7 +1932,7 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Ryan Johnson Hotel", Address = "Uritzky Street 15", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Ryan Johnson Hotel", Address = "Uritzky Street 15", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Tatarstan Hotel Complex", Address = "Pushkina Street 4", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Tatarstan Hotel Complex", Address = "Pushkina Street 4", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Courtyard by Marriott Kazan Kremlin", Address = "6 Karl Marx Street Vakhitovskiy District", City = "Kazan Russia", Stars = 4 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Courtyard by Marriott Kazan Kremlin", Address = "6 Karl Marx Street Vakhitovskiy District", City = "Kazan Russia", Stars = 4 } );</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Regina Hotel na Kirpichnikova", Address = "Akademika Kirpichnikova Street 11", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Regina Hotel na Kirpichnikova", Address = "Akademika Kirpichnikova Street 11", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Regina Na Baumana", Address = "Baumana Street 47/9", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Regina Na Baumana", Address = "Baumana Street 47/9", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="M35" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Voyage Hotel Kazan", Address = "29A Zhurnalistov", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Voyage Hotel Kazan", Address = "29A Zhurnalistov", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Safar Hotel", Address = "Odnostoronnyaya Grivka Street 1", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Safar Hotel", Address = "Odnostoronnyaya Grivka Street 1", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Shushma Hotel Kazan", Address = "Narimanov Street 15", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Shushma Hotel Kazan", Address = "Narimanov Street 15", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="M38" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Yal na Kalinina Hotel Kazan", Address = "Kalinina Street 69", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Yal na Kalinina Hotel Kazan", Address = "Kalinina Street 69", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="M39" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Kolvi Hotel", Address = "7 M Khudyakov street", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Kolvi Hotel", Address = "7 M Khudyakov street", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
       </c>
       <c r="M40" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Yal Hotel Kazan", Address = "Orenburgsky tract 20", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Yal Hotel Kazan", Address = "Orenburgsky tract 20", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="M41" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Bulak Hotel Kazan", Address = "Levobulachnaya Street 36/1", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Bulak Hotel Kazan", Address = "Levobulachnaya Street 36/1", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="M42" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Bulgar", Address = "Vishnevskogo Street 21", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel Bulgar", Address = "Vishnevskogo Street 21", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
       </c>
       <c r="M43" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Castro", Address = "Internatsionalnaya Street 1/1", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Castro", Address = "Internatsionalnaya Street 1/1", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Hills", Address = "Ayvazovskogo Street 11А", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel Hills", Address = "Ayvazovskogo Street 11А", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="M45" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Volga Hotel", Address = "Said-Galeeva Street 1", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Volga Hotel", Address = "Said-Galeeva Street 1", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="M46" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Gvardeiskaya Hotel", Address = "Gvardeiskaya Street 35", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Gvardeiskaya Hotel", Address = "Gvardeiskaya Street 35", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="M47" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel DIS Kazan", Address = "Said-Galeeva Street 25", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel DIS Kazan", Address = "Said-Galeeva Street 25", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="M48" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Hotel Aviator Kazan", Address = "Akademika Pavlova Street 1", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Hotel Aviator Kazan", Address = "Akademika Pavlova Street 1", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="M49" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Bulgaru Hostel Kazan", Address = "Universitetskaya street 4/34 Apt. 8", City = "Kazan Russia", Stars = 1 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Bulgaru Hostel Kazan", Address = "Universitetskaya street 4/34 Apt. 8", City = "Kazan Russia", Stars = 1 } );</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
       </c>
       <c r="M50" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Gorky 6 Hostel", Address = "Gorkogo Street 6", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Gorky 6 Hostel", Address = "Gorkogo Street 6", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="M51" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Fatima Hotel Kazan", Address = "Karla Marksa Street 2", City = "Kazan Russia", Stars = 3 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Fatima Hotel Kazan", Address = "Karla Marksa Street 2", City = "Kazan Russia", Stars = 3 } );</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="M52" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Vhostele", Address = "Volkova Street 54A", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Vhostele", Address = "Volkova Street 54A", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="M53" t="str">
         <f t="shared" si="0"/>
-        <v>repository.Add&lt;HotelModel&gt;(new HotelModel { Name = "Tatianin Den Hostel", Address = "Suleimanovoy Street 5", City = "Kazan Russia", Stars = 2 } );</v>
+        <v>repository.Add(new HotelModel { Name = "Tatianin Den Hostel", Address = "Suleimanovoy Street 5", City = "Kazan Russia", Stars = 2 } );</v>
       </c>
     </row>
   </sheetData>

</xml_diff>